<commit_message>
new planned place added
</commit_message>
<xml_diff>
--- a/public/python/data.xlsx
+++ b/public/python/data.xlsx
@@ -1613,7 +1613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
@@ -1915,6 +1915,23 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Iguazu Falls, Argentina</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[-25.69253235, -54.44111443902037]</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://dynamic-media-cdn.tripadvisor.com/media/photo-o/2e/ed/a5/17/foz-do-iguacu.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new coords format accepted like google maps
</commit_message>
<xml_diff>
--- a/public/python/data.xlsx
+++ b/public/python/data.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMS\Desktop\www\React_Vite\Destinero\public\python\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCD5DFD-B199-4AD0-A7A4-07E133C337BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Visited" sheetId="1" r:id="rId1"/>
-    <sheet name="Planned" sheetId="2" r:id="rId2"/>
-    <sheet name="Highlighted" sheetId="3" r:id="rId3"/>
-    <sheet name="Countries" sheetId="4" r:id="rId4"/>
+    <sheet r:id="rId1" sheetId="1" name="Visited"/>
+    <sheet r:id="rId2" sheetId="2" name="Planned"/>
+    <sheet r:id="rId3" sheetId="3" name="Highlighted"/>
+    <sheet r:id="rId4" sheetId="4" name="Countries"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -34,6 +28,15 @@
     <t>Image Links</t>
   </si>
   <si>
+    <t>Free Palestine! 🇵🇸 🍉</t>
+  </si>
+  <si>
+    <t>[31.51400376445212, 34.45846796035767]</t>
+  </si>
+  <si>
+    <t>https://img.pikbest.com/png-images/20250408/raise-the-flag-free-palestine-now_11654492.png!bw700</t>
+  </si>
+  <si>
     <t>Tokyo, Japan</t>
   </si>
   <si>
@@ -175,15 +178,6 @@
     <t>https://dynamic-media-cdn.tripadvisor.com/media/photo-o/2e/ed/a5/17/foz-do-iguacu.jpg</t>
   </si>
   <si>
-    <t>Free Palestine! 🇵🇸 🍉</t>
-  </si>
-  <si>
-    <t>[31.51400376445212, 34.45846796035767]</t>
-  </si>
-  <si>
-    <t>https://img.pikbest.com/png-images/20250408/raise-the-flag-free-palestine-now_11654492.png!bw700</t>
-  </si>
-  <si>
     <t>Auckland, New Zealand</t>
   </si>
   <si>
@@ -196,7 +190,7 @@
     <t>Jangtaesan Mountain, Daejeon</t>
   </si>
   <si>
-    <t>[36.219296, 127.3394828]</t>
+    <t>36.219296, 127.3394828</t>
   </si>
   <si>
     <t>https://blogger.googleusercontent.com/img/b/R29vZ2xl/AVvXsEgZ0QPcWXw2y6fYK9zH1uDbg-c_8ljZmnyimbGhGEgC28LB2YhvvRo8zdzaCgwfhM6WXEqfF5RZXLQOluPVeuz3245wVEXRJB_5wq47-NPdyp5gszt14kC_OdGYZBcBtDOKzG2G39oFq9IrQzPgwZeFXr4-ACbCBp1y5ypSRUKKMo-BiWbyZi8rtUUPfn7q/s856/jangtaesan.png</t>
@@ -205,7 +199,7 @@
     <t>Sky Road, Daejeon</t>
   </si>
   <si>
-    <t>[36.3271134, 127.4289631]</t>
+    <t>36.3271134, 127.4289631</t>
   </si>
   <si>
     <t>https://blogger.googleusercontent.com/img/b/R29vZ2xl/AVvXsEi7Cnm__rfxdFFhbuYl42ExWaS_lGzIqsmxNgDbWV1CwTOBtFEVGA0DZile4vugOQNSOS9lSa10cDh5u0AKHjcS9bCGsgpts7B4w6RFAaAmHUOEceMN2-1vDFO46DVvmZFFzRuQYKlQr4Zajf3dyj-5z50GIqxDMZhG_u1p8r9eGEcZoparOzD-DEcV9w2K/s2560/2.jpg</t>
@@ -214,7 +208,7 @@
     <t>Filming Site, Suncheon</t>
   </si>
   <si>
-    <t>[34.9592592, 127.5324295]</t>
+    <t>34.9592592, 127.5324295</t>
   </si>
   <si>
     <t>https://blogger.googleusercontent.com/img/b/R29vZ2xl/AVvXsEg3uS8jNtUPWLAlS7MdMi2DS0ZW9KnYB__2LkndH74DCl7crvWOQrUoBpgbe-HMPOwnIDMj1xNASITK_G81g6o1cHzNXeDJkKrHX4fbPepMQAvmTx0kjKjVeSBcY7EsccwWy9-vmDKK8otxIcXqD7Xt4az-CGgs52QW-Sq0z3y300-KPzIISuRwt3Bq6D1C/s2560/photo_2024-10-30_00-16-51.jpg</t>
@@ -802,8 +796,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -819,24 +814,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -885,44 +874,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -933,10 +937,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -974,71 +978,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1066,7 +1070,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1089,11 +1093,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1102,13 +1106,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1118,7 +1122,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1127,7 +1131,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1136,7 +1140,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1144,10 +1148,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1212,779 +1216,777 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="7" width="52.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="62.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="255.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="32.25">
+      <c r="A2" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="32.25">
+      <c r="A3" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="5" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="32.25" customFormat="1" s="3">
+      <c r="A4" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+      <c r="A12" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="21">
+      <c r="A22" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="13" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="21">
+      <c r="A24" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="13" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+      <c r="A25" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="13" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+      <c r="A26" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="21">
+      <c r="A27" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="13" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="A28" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+      <c r="A29" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+      <c r="A30" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="13" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="21">
+      <c r="A32" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="13" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="13" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="13" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+      <c r="A35" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="13" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+      <c r="A36" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+      <c r="A37" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+      <c r="A38" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+      <c r="A39" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+      <c r="A40" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="13" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="A42" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="13" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+      <c r="A43" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="13" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="A44" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="13" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+      <c r="A45" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="13" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+      <c r="A46" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="13" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="A47" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="13" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+      <c r="A48" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="13" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+      <c r="A49" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="12" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+      <c r="A50" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="12" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+      <c r="A51" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="12" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+      <c r="A52" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="12" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+      <c r="A53" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+      <c r="A54" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="12" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="A55" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="12" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="A56" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="12" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+      <c r="A57" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="12" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+      <c r="A58" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="12" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+      <c r="A59" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="A60" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="12" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="A61" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="12" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="A62" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="12" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="A63" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="12" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+      <c r="A64" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="12" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+      <c r="A65" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="12" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+      <c r="A66" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="12" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+      <c r="A67" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="12" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+      <c r="A68" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="12" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+      <c r="A69" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="12" t="s">
         <v>257</v>
       </c>
     </row>
@@ -1994,273 +1996,276 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="33.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="45.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="38.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C5" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="5" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="5" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="28.8" customFormat="1" s="3">
+      <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="28.8" customFormat="1" s="3">
+      <c r="A8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="5" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="B9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="5" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="28.8" customFormat="1" s="3">
+      <c r="A10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="B14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C16" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C17" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD1CFF5-5F34-41DF-8116-FDC82028EDD9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" customWidth="1"/>
-    <col min="3" max="3" width="106.77734375" customWidth="1"/>
+    <col min="1" max="1" style="6" width="35.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="62.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="106.7192857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2269,12 +2274,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F0A258-F35B-4FE1-A471-90C2118154B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>